<commit_message>
fine tuning for DCF
</commit_message>
<xml_diff>
--- a/src/excel/WACC_DCF_template.xlsx
+++ b/src/excel/WACC_DCF_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janko\kody\FinanceBro\src\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DABDB0-C8BB-40AB-9CE8-52533BD2F1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59E5EB7-8C7B-4755-AFC6-BF92BA7BF476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{87B14EFB-7475-4D59-A02E-613B9138E193}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{87B14EFB-7475-4D59-A02E-613B9138E193}"/>
   </bookViews>
   <sheets>
     <sheet name="WACC" sheetId="1" r:id="rId1"/>
@@ -528,7 +528,7 @@
     <xf numFmtId="169" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -634,9 +634,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -663,6 +660,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1017,21 +1018,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="21">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
     </row>
     <row r="3" spans="2:14" ht="15">
       <c r="B3" s="1"/>
@@ -1047,29 +1048,29 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="2:14" ht="15">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
     </row>
     <row r="5" spans="2:14" ht="15.6" thickBot="1">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="45"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="19" t="s">
@@ -1134,11 +1135,11 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:14" ht="15">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:14" ht="15">
@@ -1211,11 +1212,11 @@
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="2:14" ht="15">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1325,7 +1326,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6ACFC75-1EA9-47B0-896B-FB7182F3D6A4}">
   <dimension ref="B2:M23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -1335,20 +1338,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
     </row>
     <row r="3" spans="2:13" ht="15.6">
       <c r="B3" s="22"/>
@@ -1365,10 +1368,10 @@
       <c r="M3" s="23"/>
     </row>
     <row r="4" spans="2:13" ht="15.6">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="10"/>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
@@ -1381,10 +1384,10 @@
       <c r="M4" s="23"/>
     </row>
     <row r="5" spans="2:13" ht="15.6">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="45"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="10"/>
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
@@ -1416,16 +1419,16 @@
       <c r="E7" s="23"/>
       <c r="F7" s="23"/>
       <c r="G7" s="23"/>
-      <c r="H7" s="42" t="s">
+      <c r="H7" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="50" t="s">
+      <c r="I7" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
     </row>
     <row r="8" spans="2:13" ht="16.2" thickBot="1">
       <c r="B8" s="15" t="s">
@@ -1547,13 +1550,13 @@
         <v>40</v>
       </c>
       <c r="C18" s="40"/>
-      <c r="D18" s="41"/>
+      <c r="D18" s="51"/>
     </row>
     <row r="19" spans="2:4" ht="15">
       <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="32"/>
+      <c r="D19" s="50"/>
     </row>
     <row r="23" spans="2:4">
       <c r="D23" s="32"/>

</xml_diff>